<commit_message>
feat: finalizado dicionario sapataria
</commit_message>
<xml_diff>
--- a/dicionario sapataria.xlsx
+++ b/dicionario sapataria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alunos\repositories\modelagem_db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01B6A7CC-5E52-4CE4-9899-A29F1CA118DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD0143E-D1B1-4306-A00C-F9ADFB0D74C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{C402C656-23C7-49A2-859D-C12615F76A87}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="63">
   <si>
     <t>Loja de calçados e acessórios</t>
   </si>
@@ -148,6 +148,72 @@
   </si>
   <si>
     <t>DATE</t>
+  </si>
+  <si>
+    <t>cor do produto, por exemplo "azul-marinho"</t>
+  </si>
+  <si>
+    <t>preço do produto, por exemplo 1123.50</t>
+  </si>
+  <si>
+    <t>categoria, por exemplo "acessórios masculinos"</t>
+  </si>
+  <si>
+    <t>tamanho, por exemplo 43</t>
+  </si>
+  <si>
+    <t>descrição do produto em 250 caracteres</t>
+  </si>
+  <si>
+    <t>nome do produto, por exemplo "Calçado Mocassim Marrom com fivela dourada"</t>
+  </si>
+  <si>
+    <t>número para identificação e consulta</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>nome da forma de pagamento, podendo ser "débito", "crédito", "pix", "dinheiro" ou "boleto"</t>
+  </si>
+  <si>
+    <t>status da venda, podendo ser "aguardando pagamento", "pagamento aprovado", "em separação", "em trânsito" ou "entregue"</t>
+  </si>
+  <si>
+    <t>nome do cliente</t>
+  </si>
+  <si>
+    <t>telefone no formato brasileiro sem DDI, por exemplo "15987654321"</t>
+  </si>
+  <si>
+    <t>endereço de entrega completo, por exemplo "Estrada do Dinorah, 1815, Quadra S, Lote 11 - Parque São Bento 18071-036"</t>
+  </si>
+  <si>
+    <t>email do cliente, por exemplo "central+de+relacionamento+e+compras@secretariadeurbanismo.sp.gov.br"</t>
+  </si>
+  <si>
+    <t>data da realização da compra</t>
+  </si>
+  <si>
+    <t>valor total da soma dos produtos comprados</t>
+  </si>
+  <si>
+    <t>número para identificação e consulta na tabela Cliente</t>
+  </si>
+  <si>
+    <t>número para identificação e consulta na tabela Produto</t>
+  </si>
+  <si>
+    <t>número para identificação e consulta na tabela Venda</t>
+  </si>
+  <si>
+    <t>número para identificação e consulta na tabela Estoque</t>
+  </si>
+  <si>
+    <t>quantidade de itens disponíveis para um produto específico em um estoque específico</t>
+  </si>
+  <si>
+    <t>nome do local do estoque, por exemplo "Galpão 3 Girasol em Holambra/SP"</t>
   </si>
 </sst>
 </file>
@@ -294,6 +360,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,13 +382,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,49 +707,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6981007-03C4-448A-AF72-A4C2E9F20287}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6.453125" customWidth="1"/>
     <col min="2" max="2" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="108.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -688,7 +760,9 @@
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>37</v>
       </c>
@@ -701,7 +775,9 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>38</v>
       </c>
@@ -714,12 +790,14 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="1">
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -727,12 +805,14 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E7" s="1">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -740,37 +820,39 @@
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E8" s="2">
-        <v>50</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -781,7 +863,9 @@
       <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>37</v>
       </c>
@@ -794,105 +878,131 @@
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="13"/>
+      <c r="E12" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1">
+        <v>250</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="12" t="s">
+      <c r="B19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="13">
         <v>6</v>
       </c>
     </row>
@@ -901,44 +1011,60 @@
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="D21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="11" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="D22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="11">
+        <v>8</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="D23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="11">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="11">
+        <v>20</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
@@ -947,104 +1073,114 @@
       <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="D25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="12">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9" t="s">
+      <c r="C28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="3">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="12">
+        <v>50</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="12" t="s">
+      <c r="B31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9" t="s">
+      <c r="C32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="3">
         <v>6</v>
       </c>
     </row>
@@ -1055,7 +1191,9 @@
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="D33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1064,43 +1202,45 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="12" t="s">
+      <c r="B35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="E35" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9" t="s">
+      <c r="C36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="3">
         <v>6</v>
       </c>
     </row>
@@ -1111,7 +1251,9 @@
       <c r="B37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="D37" s="1" t="s">
         <v>37</v>
       </c>
@@ -1124,7 +1266,9 @@
       <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="D38" s="2" t="s">
         <v>37</v>
       </c>

</xml_diff>